<commit_message>
fix PlainExcelGenerator for DateOnly and TimeOnly
</commit_message>
<xml_diff>
--- a/Signum.Engine.Extensions/Excel/plainExcelTemplate.xlsx
+++ b/Signum.Engine.Extensions/Excel/plainExcelTemplate.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\IntTec\Extensions\Signum.Engine.Extensions\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Agile360\Framework\Signum.Engine.Extensions\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061F9062-C7B1-491F-9C79-56185E9D402F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="60" windowWidth="20115" windowHeight="10515"/>
+    <workbookView xWindow="2985" yWindow="5085" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>HeaderCell</t>
   </si>
@@ -46,20 +58,23 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>Hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="[$¥-804]#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="[$£-809]#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="[$$-409]#,##0.00"/>
-    <numFmt numFmtId="170" formatCode="0&quot; km&quot;"/>
+    <numFmt numFmtId="166" formatCode="[$¥-804]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="0&quot; km&quot;"/>
+    <numFmt numFmtId="171" formatCode="[$-F400]h:mm:ss\ am/pm"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -137,18 +152,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Prozent" xfId="4" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="2" builtinId="15"/>
-    <cellStyle name="Überschrift 2" xfId="1" builtinId="17"/>
-    <cellStyle name="Währung" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
+    <cellStyle name="Title" xfId="2" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -164,7 +179,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -239,6 +254,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -274,6 +306,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -449,14 +498,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
@@ -491,6 +540,9 @@
       <c r="H2" t="s">
         <v>8</v>
       </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
@@ -509,52 +561,54 @@
       <c r="G3" s="5">
         <v>12</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="13">
         <v>0.2</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="14">
+        <v>0.5</v>
+      </c>
       <c r="J3" s="11"/>
       <c r="K3" s="10"/>
-      <c r="L3" s="13"/>
+      <c r="L3" s="12"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L4" s="13"/>
+      <c r="L4" s="12"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L5" s="13"/>
+      <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L6" s="13"/>
+      <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L7" s="13"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L8" s="13"/>
+      <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L9" s="13"/>
+      <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L10" s="13"/>
+      <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L11" s="13"/>
+      <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L12" s="13"/>
+      <c r="L12" s="12"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L13" s="13"/>
+      <c r="L13" s="12"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L14" s="13"/>
+      <c r="L14" s="12"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L15" s="13"/>
+      <c r="L15" s="12"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L16" s="13"/>
+      <c r="L16" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish ImportFromExcel (except for MList)
</commit_message>
<xml_diff>
--- a/Signum.Engine.Extensions/Excel/plainExcelTemplate.xlsx
+++ b/Signum.Engine.Extensions/Excel/plainExcelTemplate.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Agile360\Framework\Signum.Engine.Extensions\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Signum\southwind\Framework\Signum.Engine.Extensions\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061F9062-C7B1-491F-9C79-56185E9D402F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="5085" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="5085" windowWidth="21600" windowHeight="12735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>HeaderCell</t>
   </si>
@@ -61,20 +60,23 @@
   </si>
   <si>
     <t>Hour</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="[$¥-804]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="0&quot; km&quot;"/>
-    <numFmt numFmtId="171" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+    <numFmt numFmtId="168" formatCode="0&quot; km&quot;"/>
+    <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -154,9 +156,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
@@ -254,23 +256,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -306,23 +291,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -498,24 +466,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="22.5" x14ac:dyDescent="0.6">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,10 +511,12 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="9"/>
+      <c r="J2" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B3" s="2">
         <v>31361</v>
       </c>
@@ -567,47 +537,49 @@
       <c r="I3" s="14">
         <v>0.5</v>
       </c>
-      <c r="J3" s="11"/>
+      <c r="J3" s="11" t="b">
+        <v>0</v>
+      </c>
       <c r="K3" s="10"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L16" s="12"/>
     </row>
   </sheetData>

</xml_diff>